<commit_message>
Thêm phần khung cho phần lấy tỷ giá và phần thực hiện giao dịch với API của bên Thứ 3
</commit_message>
<xml_diff>
--- a/docs/Sprint 4 - 0504 To 1904/LogTime.xlsx
+++ b/docs/Sprint 4 - 0504 To 1904/LogTime.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OTHER\Project-e\Github\docs\Sprint 4 - 0504 To 1904\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
     <sheet name="ANHDT" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,9 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>4/7/2014</t>
+  </si>
+  <si>
+    <t>4/8/2014</t>
+  </si>
+  <si>
+    <t>4/9/2014</t>
+  </si>
+  <si>
+    <t>4/10/2014</t>
+  </si>
+  <si>
+    <t>4/11/2014</t>
+  </si>
+  <si>
+    <t>4/12/2014</t>
+  </si>
+  <si>
+    <t>4/13/2014</t>
+  </si>
+  <si>
+    <t>4/14/2014</t>
+  </si>
+  <si>
+    <t>4/15/2014</t>
+  </si>
+  <si>
+    <t>4/16/2014</t>
+  </si>
+  <si>
+    <t>4/17/2014</t>
+  </si>
+  <si>
+    <t>4/18/2014</t>
+  </si>
+  <si>
+    <t>4/19/2014</t>
+  </si>
+  <si>
+    <t>4/20/2014</t>
+  </si>
+  <si>
+    <t>Payment - Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment - model </t>
+  </si>
+  <si>
+    <t>Refactor : model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin Login page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">và cơ chế phân biệt giữa user và admin </t>
+  </si>
+  <si>
+    <t>Update login subsystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metting + Quản lý team task </t>
+  </si>
+  <si>
+    <t>Hoàn thành PIN, có thể pin từ product/details/1. trong pin ta có thể làm movetocart, movetowishlist, remove mà không cần load lại trang</t>
+  </si>
+  <si>
+    <t>Chat</t>
   </si>
 </sst>
 </file>
@@ -63,14 +127,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -81,6 +155,110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O10" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:O10"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="4/7/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/7/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="4/8/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/8/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="4/9/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/9/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="4/10/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/10/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="4/11/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/11/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="4/12/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/12/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="4/13/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/13/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="4/14/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/14/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="4/15/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/15/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="4/16/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/16/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" name="4/17/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/17/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" name="4/18/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/18/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" name="4/19/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/19/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="15" name="4/20/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[4/20/2014])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:O10" totalsRowCount="1" headerRowDxfId="0">
+  <autoFilter ref="A1:O9"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="4/7/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/7/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="4/8/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/8/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="4/9/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/9/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="4/10/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/10/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="4/11/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/11/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="4/12/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/12/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="4/13/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/13/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="4/14/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/14/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="4/15/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/15/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="4/16/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/16/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" name="4/17/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/17/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" name="4/18/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/18/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" name="4/19/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/19/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="15" name="4/20/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[4/20/2014])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -126,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +339,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,7 +516,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -346,15 +524,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
@@ -367,63 +545,189 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>41736</v>
-      </c>
-      <c r="C1" s="1">
-        <v>41737</v>
-      </c>
-      <c r="D1" s="1">
-        <v>41738</v>
-      </c>
-      <c r="E1" s="1">
-        <v>41739</v>
-      </c>
-      <c r="F1" s="1">
-        <v>41740</v>
-      </c>
-      <c r="G1" s="1">
-        <v>41741</v>
-      </c>
-      <c r="H1" s="1">
-        <v>41742</v>
-      </c>
-      <c r="I1" s="1">
-        <v>41743</v>
-      </c>
-      <c r="J1" s="1">
-        <v>41744</v>
-      </c>
-      <c r="K1" s="1">
-        <v>41745</v>
-      </c>
-      <c r="L1" s="1">
-        <v>41746</v>
-      </c>
-      <c r="M1" s="1">
-        <v>41747</v>
-      </c>
-      <c r="N1" s="1">
-        <v>41748</v>
-      </c>
-      <c r="O1" s="1">
-        <v>41749</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>SUM(Table2[4/7/2014])</f>
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <f>SUM(Table2[4/8/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>SUM(Table2[4/9/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f>SUM(Table2[4/10/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f>SUM(Table2[4/11/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <f>SUM(Table2[4/12/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>SUM(Table2[4/13/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUM(Table2[4/14/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f>SUM(Table2[4/15/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>SUM(Table2[4/16/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>SUM(Table2[4/17/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>SUM(Table2[4/18/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>SUM(Table2[4/19/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>SUM(Table2[4/20/2014])</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,8 +738,133 @@
     <col min="9" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.28515625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>SUM(Table24[4/7/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>SUM(Table24[4/8/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>SUM(Table24[4/9/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>SUM(Table24[4/10/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>SUM(Table24[4/11/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>SUM(Table24[4/12/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>SUM(Table24[4/13/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUM(Table24[4/14/2014])</f>
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <f>SUM(Table24[4/15/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>SUM(Table24[4/16/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>SUM(Table24[4/17/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>SUM(Table24[4/18/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>SUM(Table24[4/19/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>SUM(Table24[4/20/2014])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit baseline UI home
</commit_message>
<xml_diff>
--- a/docs/Sprint 4 - 0504 To 1904/LogTime.xlsx
+++ b/docs/Sprint 4 - 0504 To 1904/LogTime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>Chat</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Payment History</t>
+  </si>
+  <si>
+    <t>Thiết kế Process từ place order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">payment </t>
+  </si>
+  <si>
+    <t>Issue confict cookie</t>
+  </si>
+  <si>
+    <t>Add sản phẩm cho admin</t>
   </si>
 </sst>
 </file>
@@ -139,10 +157,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O10" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:O10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O12" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:O11"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="4/7/2014" totalsRowFunction="custom">
@@ -516,7 +534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +619,9 @@
       <c r="I2">
         <v>2</v>
       </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -656,62 +677,101 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+    </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12">
         <f>SUM(Table2[4/7/2014])</f>
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <f>SUM(Table2[4/8/2014])</f>
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <f>SUM(Table2[4/9/2014])</f>
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <f>SUM(Table2[4/10/2014])</f>
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <f>SUM(Table2[4/11/2014])</f>
         <v>4</v>
       </c>
-      <c r="G10">
+      <c r="G12">
         <f>SUM(Table2[4/12/2014])</f>
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H12">
         <f>SUM(Table2[4/13/2014])</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I12">
         <f>SUM(Table2[4/14/2014])</f>
         <v>4</v>
       </c>
-      <c r="J10">
+      <c r="J12">
         <f>SUM(Table2[4/15/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="K12">
         <f>SUM(Table2[4/16/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="L12">
         <f>SUM(Table2[4/17/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="M12">
         <f>SUM(Table2[4/18/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="N12">
         <f>SUM(Table2[4/19/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="O12">
         <f>SUM(Table2[4/20/2014])</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -726,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +861,39 @@
       <c r="I3">
         <v>8</v>
       </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -837,27 +930,27 @@
       </c>
       <c r="J10">
         <f>SUM(Table24[4/15/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <f>SUM(Table24[4/16/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L10">
         <f>SUM(Table24[4/17/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M10">
         <f>SUM(Table24[4/18/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10">
         <f>SUM(Table24[4/19/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O10">
         <f>SUM(Table24[4/20/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>